<commit_message>
Added in more examples
This is still a work in progress
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/7_Text_Functions.xlsx
+++ b/2_Formulas_Functions/7_Text_Functions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1D2DFD-7497-4E48-ADAD-61A3C2A6C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66509367-26E6-49F8-9D4E-CFCDCE4C6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original_Luke" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="66">
   <si>
     <t>Email</t>
   </si>
@@ -227,6 +250,15 @@
   </si>
   <si>
     <t>meredith.palmer@outlook.com</t>
+  </si>
+  <si>
+    <t>Full Address</t>
+  </si>
+  <si>
+    <t>Unique Jobs</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -411,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -426,6 +458,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BCB134-41DE-47D5-9456-1C60C9867AFA}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,9 +1264,10 @@
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1255,8 +1289,11 @@
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
@@ -1278,8 +1315,12 @@
       <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,E2,F2)</f>
+        <v>457 Oak St San Jose, CA, 95101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
@@ -1301,8 +1342,12 @@
       <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I21" si="0">_xlfn.TEXTJOIN(" ",TRUE,E3,F3)</f>
+        <v>203 Birch St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -1324,8 +1369,12 @@
       <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>790 Pine St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -1347,8 +1396,12 @@
       <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>457 Oak St San Jose, CA, 95101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
@@ -1370,8 +1423,12 @@
       <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>459 Oak St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -1393,8 +1450,12 @@
       <c r="G7" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>204 Birch St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>59</v>
       </c>
@@ -1416,8 +1477,12 @@
       <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>790 Pine St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -1439,8 +1504,12 @@
       <c r="G9" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>204 Birch St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -1462,8 +1531,12 @@
       <c r="G10" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>123 Elm St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1485,8 +1558,12 @@
       <c r="G11" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>123 Elm St Los Angeles, CA, 90001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1508,8 +1585,12 @@
       <c r="G12" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>123 Elm St San Diego, CA, 92101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -1531,8 +1612,12 @@
       <c r="G13" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>202 Birch St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1554,8 +1639,12 @@
       <c r="G14" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>204 Birch St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
@@ -1577,8 +1666,12 @@
       <c r="G15" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>123 Elm St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
@@ -1600,8 +1693,12 @@
       <c r="G16" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>456 Oak St Chicago, IL, 60601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1623,8 +1720,12 @@
       <c r="G17" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>203 Birch St Chicago, IL, 60602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1646,8 +1747,12 @@
       <c r="G18" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>459 Oak St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
@@ -1669,8 +1774,12 @@
       <c r="G19" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>456 Oak St New York, NY, 10001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1692,8 +1801,12 @@
       <c r="G20" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>459 Oak St Philadelphia, PA, 19101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1714,6 +1827,10 @@
       </c>
       <c r="G21" s="9" t="s">
         <v>10</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>459 Oak St New York, NY, 10001</v>
       </c>
     </row>
   </sheetData>
@@ -1723,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F197DD-EE87-4022-A4E6-1027B6E64DD6}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,12 +1852,539 @@
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="10" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>45505</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2:I6">_xlfn.UNIQUE(B2:B21)</f>
+        <v>Data Analyst</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11">
+        <v>45506</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Business Intelligence Analyst</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="11">
+        <v>45508</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Data Engineer</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>45509</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Data Scientist</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="11">
+        <v>45511</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Machine Learning Engineer</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11">
+        <v>45512</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11">
+        <v>45514</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>45516</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="11">
+        <v>45517</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11">
+        <v>45519</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11">
+        <v>45520</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11">
+        <v>45522</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11">
+        <v>45523</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="11">
+        <v>45525</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11">
+        <v>45527</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="11">
+        <v>45528</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="11">
+        <v>45530</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="11">
+        <v>45531</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="11">
+        <v>45533</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="13">
+        <v>45535</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E73CB36-69AF-4B27-BCC8-FDB353A4DE72}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1762,8 +2406,11 @@
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
@@ -1785,8 +2432,12 @@
       <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="str">
+        <f>RIGHT(F2,9)</f>
+        <v>CA, 95101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +2460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -1832,7 +2483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -1855,7 +2506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
@@ -1878,7 +2529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -1901,7 +2552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>59</v>
       </c>
@@ -1924,7 +2575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -1947,7 +2598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -1970,7 +2621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1993,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
@@ -2016,7 +2667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2039,7 +2690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2062,7 +2713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
@@ -2085,7 +2736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Create Date and Time File
And update Text Functions
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/7_Text_Functions.xlsx
+++ b/2_Formulas_Functions/7_Text_Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6EE17C-6C3C-43D6-BF92-ED8D4412584D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81899903-EEAF-4F26-BBDD-BA8A73258393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -522,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -538,14 +538,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1786,7 +1782,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2398,6 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="18"/>
       <c r="J1" s="13" t="s">
         <v>63</v>
       </c>
@@ -2432,7 +2427,6 @@
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="17"/>
       <c r="J2" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,F2,G2)</f>
         <v>457 Oak St San Jose, CA, 95101</v>
@@ -2463,7 +2457,6 @@
       <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="17"/>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J21" si="0">_xlfn.TEXTJOIN(" ",TRUE,F3,G3)</f>
         <v>203 Birch St Chicago, IL, 60601</v>
@@ -2494,7 +2487,6 @@
       <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17"/>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>790 Pine St Chicago, IL, 60601</v>
@@ -2525,7 +2517,6 @@
       <c r="H5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="17"/>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>457 Oak St San Jose, CA, 95101</v>
@@ -2556,7 +2547,6 @@
       <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="17"/>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
         <v>459 Oak St Philadelphia, PA, 19101</v>
@@ -2587,7 +2577,6 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="17"/>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
         <v>204 Birch St Philadelphia, PA, 19101</v>
@@ -2618,7 +2607,6 @@
       <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="17"/>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
         <v>790 Pine St Chicago, IL, 60601</v>
@@ -2649,7 +2637,6 @@
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="17"/>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
         <v>204 Birch St Philadelphia, PA, 19101</v>
@@ -2680,7 +2667,6 @@
       <c r="H10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="17"/>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
         <v>123 Elm St Chicago, IL, 60601</v>
@@ -2711,7 +2697,6 @@
       <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="17"/>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
         <v>123 Elm St Los Angeles, CA, 90001</v>
@@ -2742,7 +2727,6 @@
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="17"/>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
         <v>123 Elm St San Diego, CA, 92101</v>
@@ -2773,7 +2757,6 @@
       <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="17"/>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
         <v>202 Birch St Chicago, IL, 60601</v>
@@ -2804,7 +2787,6 @@
       <c r="H14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="17"/>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
         <v>204 Birch St Philadelphia, PA, 19101</v>
@@ -2835,7 +2817,6 @@
       <c r="H15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="17"/>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
         <v>123 Elm St Chicago, IL, 60601</v>
@@ -2866,7 +2847,6 @@
       <c r="H16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="17"/>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
         <v>456 Oak St Chicago, IL, 60601</v>
@@ -2897,7 +2877,6 @@
       <c r="H17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="17"/>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
         <v>203 Birch St Chicago, IL, 60602</v>
@@ -2928,7 +2907,6 @@
       <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="17"/>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
         <v>459 Oak St Philadelphia, PA, 19101</v>
@@ -2959,7 +2937,6 @@
       <c r="H19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="17"/>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
         <v>456 Oak St New York, NY, 10001</v>
@@ -2990,7 +2967,6 @@
       <c r="H20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="17"/>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
         <v>459 Oak St Philadelphia, PA, 19101</v>
@@ -3021,7 +2997,6 @@
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="17"/>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
         <v>459 Oak St New York, NY, 10001</v>
@@ -3087,14 +3062,14 @@
       <c r="J1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="13" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3986,12 +3961,11 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -4018,16 +3992,15 @@
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="20">
+      <c r="J2">
         <f>FIND(", ", G2)+1</f>
         <v>10</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2">
         <f>FIND(", ", G2, J2)</f>
         <v>13</v>
       </c>
-      <c r="L2" s="20" t="str">
+      <c r="L2" t="str">
         <f>MID(G2,J2+1,K2-J2-1)</f>
         <v>CA</v>
       </c>
@@ -4057,16 +4030,15 @@
       <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="20">
+      <c r="J3">
         <f t="shared" ref="J3:J21" si="0">FIND(", ", G3)+1</f>
         <v>9</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3">
         <f t="shared" ref="K3:K21" si="1">FIND(", ", G3, J3)</f>
         <v>12</v>
       </c>
-      <c r="L3" s="20" t="str">
+      <c r="L3" t="str">
         <f t="shared" ref="L3:L21" si="2">MID(G3,J3+1,K3-J3-1)</f>
         <v>IL</v>
       </c>
@@ -4096,16 +4068,15 @@
       <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="20">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L4" s="20" t="str">
+      <c r="L4" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4135,16 +4106,15 @@
       <c r="H5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="20">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L5" s="20" t="str">
+      <c r="L5" t="str">
         <f t="shared" si="2"/>
         <v>CA</v>
       </c>
@@ -4174,16 +4144,15 @@
       <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="20">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L6" s="20" t="str">
+      <c r="L6" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4213,16 +4182,15 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="20">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L7" s="20" t="str">
+      <c r="L7" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4252,16 +4220,15 @@
       <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="20">
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L8" s="20" t="str">
+      <c r="L8" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4291,16 +4258,15 @@
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="20">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="20" t="str">
+      <c r="L9" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4330,16 +4296,15 @@
       <c r="H10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="20">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L10" s="20" t="str">
+      <c r="L10" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4369,16 +4334,15 @@
       <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="20">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L11" s="20" t="str">
+      <c r="L11" t="str">
         <f t="shared" si="2"/>
         <v>CA</v>
       </c>
@@ -4408,16 +4372,15 @@
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="20">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="L12" s="20" t="str">
+      <c r="L12" t="str">
         <f t="shared" si="2"/>
         <v>CA</v>
       </c>
@@ -4447,16 +4410,15 @@
       <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="20">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L13" s="20" t="str">
+      <c r="L13" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4486,16 +4448,15 @@
       <c r="H14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="20">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L14" s="20" t="str">
+      <c r="L14" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4525,16 +4486,15 @@
       <c r="H15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="20">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L15" s="20" t="str">
+      <c r="L15" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4564,16 +4524,15 @@
       <c r="H16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="20">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L16" s="20" t="str">
+      <c r="L16" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4603,16 +4562,15 @@
       <c r="H17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="20">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L17" s="20" t="str">
+      <c r="L17" t="str">
         <f t="shared" si="2"/>
         <v>IL</v>
       </c>
@@ -4642,16 +4600,15 @@
       <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="20">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L18" s="20" t="str">
+      <c r="L18" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4681,16 +4638,15 @@
       <c r="H19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="20">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L19" s="20" t="str">
+      <c r="L19" t="str">
         <f t="shared" si="2"/>
         <v>NY</v>
       </c>
@@ -4720,16 +4676,15 @@
       <c r="H20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="20">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L20" s="20" t="str">
+      <c r="L20" t="str">
         <f t="shared" si="2"/>
         <v>PA</v>
       </c>
@@ -4759,16 +4714,15 @@
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="20">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L21" s="20" t="str">
+      <c r="L21" t="str">
         <f t="shared" si="2"/>
         <v>NY</v>
       </c>

</xml_diff>

<commit_message>
Update Application Date & Time Column
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/7_Text_Functions.xlsx
+++ b/2_Formulas_Functions/7_Text_Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C04C014-F11F-4C69-BF57-AE87F8B6E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB0F12E-2AB8-4E59-8773-8021B550FDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -540,11 +540,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1785,7 +1785,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="M30" sqref="M30:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1836,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>44971.640277777777</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1862,8 +1862,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15">
-        <v>45055.406597222223</v>
+      <c r="D3" s="14">
+        <v>45055.40625</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -1888,8 +1888,8 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15">
-        <v>45128.770833333336</v>
+      <c r="D4" s="14">
+        <v>45128.729166666664</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -1914,8 +1914,8 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
-        <v>45173.302604166667</v>
+      <c r="D5" s="14">
+        <v>45173.302083333336</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -1940,8 +1940,8 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
-        <v>45248.833333333336</v>
+      <c r="D6" s="14">
+        <v>45248.708333333336</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -1966,8 +1966,8 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15">
-        <v>45302.531423611108</v>
+      <c r="D7" s="14">
+        <v>45302.53125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -1992,8 +1992,8 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
-        <v>45354.687847222223</v>
+      <c r="D8" s="14">
+        <v>45354.6875</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -2018,7 +2018,7 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45408.340277777781</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2044,8 +2044,8 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15">
-        <v>45458.806076388886</v>
+      <c r="D10" s="14">
+        <v>45458.743055555555</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -2070,7 +2070,7 @@
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>45480.607638888891</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2096,8 +2096,8 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15">
-        <v>45455.285069444442</v>
+      <c r="D12" s="14">
+        <v>45455.284722222219</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -2122,7 +2122,7 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>44951.552083333336</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2148,8 +2148,8 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15">
-        <v>45002.490104166667</v>
+      <c r="D14" s="14">
+        <v>45002.489583333336</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -2174,7 +2174,7 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>45078.416666666664</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2200,8 +2200,8 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="15">
-        <v>45168.937673611108</v>
+      <c r="D16" s="14">
+        <v>45168.729166666664</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -2226,8 +2226,8 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="15">
-        <v>45218.236458333333</v>
+      <c r="D17" s="14">
+        <v>45218.319444444445</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -2252,7 +2252,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>45350.71875</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2278,8 +2278,8 @@
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15">
-        <v>45418.892881944441</v>
+      <c r="D19" s="14">
+        <v>45418.725694444445</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -2304,8 +2304,8 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>45496.083333333336</v>
+      <c r="D20" s="14">
+        <v>45496.291666666664</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -2330,8 +2330,8 @@
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16">
-        <v>45422.989930555559</v>
+      <c r="D21" s="15">
+        <v>45422.739583333336</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -2360,7 +2360,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D21"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2415,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>44971.640277777777</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -2445,8 +2445,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15">
-        <v>45055.406597222223</v>
+      <c r="D3" s="14">
+        <v>45055.40625</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -2475,8 +2475,8 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15">
-        <v>45128.770833333336</v>
+      <c r="D4" s="14">
+        <v>45128.729166666664</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -2505,8 +2505,8 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
-        <v>45173.302604166667</v>
+      <c r="D5" s="14">
+        <v>45173.302083333336</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -2535,8 +2535,8 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
-        <v>45248.833333333336</v>
+      <c r="D6" s="14">
+        <v>45248.708333333336</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -2565,8 +2565,8 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15">
-        <v>45302.531423611108</v>
+      <c r="D7" s="14">
+        <v>45302.53125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -2595,8 +2595,8 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
-        <v>45354.687847222223</v>
+      <c r="D8" s="14">
+        <v>45354.6875</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -2625,7 +2625,7 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45408.340277777781</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2655,8 +2655,8 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15">
-        <v>45458.806076388886</v>
+      <c r="D10" s="14">
+        <v>45458.743055555555</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -2685,7 +2685,7 @@
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>45480.607638888891</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2715,8 +2715,8 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15">
-        <v>45455.285069444442</v>
+      <c r="D12" s="14">
+        <v>45455.284722222219</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -2745,7 +2745,7 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>44951.552083333336</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2775,8 +2775,8 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15">
-        <v>45002.490104166667</v>
+      <c r="D14" s="14">
+        <v>45002.489583333336</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -2805,7 +2805,7 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>45078.416666666664</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2835,8 +2835,8 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="15">
-        <v>45168.937673611108</v>
+      <c r="D16" s="14">
+        <v>45168.729166666664</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -2865,8 +2865,8 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="15">
-        <v>45218.236458333333</v>
+      <c r="D17" s="14">
+        <v>45218.319444444445</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -2895,7 +2895,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>45350.71875</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2925,8 +2925,8 @@
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15">
-        <v>45418.892881944441</v>
+      <c r="D19" s="14">
+        <v>45418.725694444445</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -2955,8 +2955,8 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>45496.083333333336</v>
+      <c r="D20" s="14">
+        <v>45496.291666666664</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -2985,8 +2985,8 @@
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16">
-        <v>45422.989930555559</v>
+      <c r="D21" s="15">
+        <v>45422.739583333336</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -3015,7 +3015,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D21"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,7 +3086,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>44971.640277777777</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -3131,8 +3131,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15">
-        <v>45055.406597222223</v>
+      <c r="D3" s="14">
+        <v>45055.40625</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -3175,8 +3175,8 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15">
-        <v>45128.770833333336</v>
+      <c r="D4" s="14">
+        <v>45128.729166666664</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -3219,8 +3219,8 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
-        <v>45173.302604166667</v>
+      <c r="D5" s="14">
+        <v>45173.302083333336</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -3263,8 +3263,8 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
-        <v>45248.833333333336</v>
+      <c r="D6" s="14">
+        <v>45248.708333333336</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -3307,8 +3307,8 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15">
-        <v>45302.531423611108</v>
+      <c r="D7" s="14">
+        <v>45302.53125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -3348,8 +3348,8 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
-        <v>45354.687847222223</v>
+      <c r="D8" s="14">
+        <v>45354.6875</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -3389,7 +3389,7 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45408.340277777781</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -3430,8 +3430,8 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15">
-        <v>45458.806076388886</v>
+      <c r="D10" s="14">
+        <v>45458.743055555555</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -3471,7 +3471,7 @@
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>45480.607638888891</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -3512,8 +3512,8 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15">
-        <v>45455.285069444442</v>
+      <c r="D12" s="14">
+        <v>45455.284722222219</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -3553,7 +3553,7 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>44951.552083333336</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -3594,8 +3594,8 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15">
-        <v>45002.490104166667</v>
+      <c r="D14" s="14">
+        <v>45002.489583333336</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -3635,7 +3635,7 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>45078.416666666664</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -3676,8 +3676,8 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="15">
-        <v>45168.937673611108</v>
+      <c r="D16" s="14">
+        <v>45168.729166666664</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -3717,8 +3717,8 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="15">
-        <v>45218.236458333333</v>
+      <c r="D17" s="14">
+        <v>45218.319444444445</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -3758,7 +3758,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>45350.71875</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -3799,8 +3799,8 @@
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15">
-        <v>45418.892881944441</v>
+      <c r="D19" s="14">
+        <v>45418.725694444445</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -3840,8 +3840,8 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>45496.083333333336</v>
+      <c r="D20" s="14">
+        <v>45496.291666666664</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -3881,8 +3881,8 @@
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16">
-        <v>45422.989930555559</v>
+      <c r="D21" s="15">
+        <v>45422.739583333336</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -3922,7 +3922,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,11 +3964,11 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3980,7 +3980,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>44971.640277777777</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -4018,8 +4018,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15">
-        <v>45055.406597222223</v>
+      <c r="D3" s="14">
+        <v>45055.40625</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -4056,8 +4056,8 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15">
-        <v>45128.770833333336</v>
+      <c r="D4" s="14">
+        <v>45128.729166666664</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -4094,8 +4094,8 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
-        <v>45173.302604166667</v>
+      <c r="D5" s="14">
+        <v>45173.302083333336</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -4132,8 +4132,8 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
-        <v>45248.833333333336</v>
+      <c r="D6" s="14">
+        <v>45248.708333333336</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -4170,8 +4170,8 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15">
-        <v>45302.531423611108</v>
+      <c r="D7" s="14">
+        <v>45302.53125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -4208,8 +4208,8 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
-        <v>45354.687847222223</v>
+      <c r="D8" s="14">
+        <v>45354.6875</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -4246,7 +4246,7 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45408.340277777781</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -4284,8 +4284,8 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15">
-        <v>45458.806076388886</v>
+      <c r="D10" s="14">
+        <v>45458.743055555555</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -4322,7 +4322,7 @@
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>45480.607638888891</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -4360,8 +4360,8 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15">
-        <v>45455.285069444442</v>
+      <c r="D12" s="14">
+        <v>45455.284722222219</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -4398,7 +4398,7 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>44951.552083333336</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -4436,8 +4436,8 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15">
-        <v>45002.490104166667</v>
+      <c r="D14" s="14">
+        <v>45002.489583333336</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -4474,7 +4474,7 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>45078.416666666664</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -4512,8 +4512,8 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="15">
-        <v>45168.937673611108</v>
+      <c r="D16" s="14">
+        <v>45168.729166666664</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -4550,8 +4550,8 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="15">
-        <v>45218.236458333333</v>
+      <c r="D17" s="14">
+        <v>45218.319444444445</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -4588,7 +4588,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>45350.71875</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -4626,8 +4626,8 @@
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15">
-        <v>45418.892881944441</v>
+      <c r="D19" s="14">
+        <v>45418.725694444445</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -4664,8 +4664,8 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>45496.083333333336</v>
+      <c r="D20" s="14">
+        <v>45496.291666666664</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -4702,8 +4702,8 @@
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16">
-        <v>45422.989930555559</v>
+      <c r="D21" s="15">
+        <v>45422.739583333336</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added in time examples
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/7_Text_Functions.xlsx
+++ b/2_Formulas_Functions/7_Text_Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D707D5D-20BF-4807-B991-130EA48C94C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B5D68-5AAA-4534-8755-FEC7F13B1F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,8 +540,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30:N30"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>44971.640277777777</v>
+        <v>44971.640451388892</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
@@ -1862,7 +1862,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="12">
-        <v>45055.40625</v>
+        <v>45055.40662037037</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -1888,7 +1888,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12">
-        <v>45128.729166666664</v>
+        <v>45128.729710648149</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -1914,7 +1914,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="12">
-        <v>45173.302083333336</v>
+        <v>45173.302187499998</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -1940,7 +1940,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="12">
-        <v>45248.708333333336</v>
+        <v>45248.70857638889</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -1966,7 +1966,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="12">
-        <v>45302.53125</v>
+        <v>45302.531921296293</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -1992,7 +1992,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="12">
-        <v>45354.6875</v>
+        <v>45354.687881944446</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -2018,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12">
-        <v>45408.340277777781</v>
+        <v>45408.340810185182</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>47</v>
@@ -2044,7 +2044,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="12">
-        <v>45458.743055555555</v>
+        <v>45458.743333333332</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -2070,7 +2070,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="12">
-        <v>45480.607638888891</v>
+        <v>45480.608055555553</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
@@ -2096,7 +2096,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="12">
-        <v>45455.284722222219</v>
+        <v>45455.284930555557</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -2122,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="12">
-        <v>44951.552083333336</v>
+        <v>44951.552141203705</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>57</v>
@@ -2148,7 +2148,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="12">
-        <v>45002.489583333336</v>
+        <v>45002.490034722221</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -2174,7 +2174,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="12">
-        <v>45078.416666666664</v>
+        <v>45078.417256944442</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>53</v>
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="12">
-        <v>45168.729166666664</v>
+        <v>45168.729328703703</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -2226,7 +2226,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="12">
-        <v>45218.319444444445</v>
+        <v>45218.319780092592</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -2252,7 +2252,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="12">
-        <v>45350.71875</v>
+        <v>45350.719236111108</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -2278,7 +2278,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="12">
-        <v>45418.725694444445</v>
+        <v>45418.726354166669</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -2304,7 +2304,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="12">
-        <v>45496.291666666664</v>
+        <v>45496.291701388887</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -2330,7 +2330,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="13">
-        <v>45422.739583333336</v>
+        <v>45422.739884259259</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -2359,7 +2359,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>44971.640277777777</v>
+        <v>44971.640451388892</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
@@ -2445,7 +2445,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="12">
-        <v>45055.40625</v>
+        <v>45055.40662037037</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -2475,7 +2475,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12">
-        <v>45128.729166666664</v>
+        <v>45128.729710648149</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -2505,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="12">
-        <v>45173.302083333336</v>
+        <v>45173.302187499998</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -2535,7 +2535,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="12">
-        <v>45248.708333333336</v>
+        <v>45248.70857638889</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -2565,7 +2565,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="12">
-        <v>45302.53125</v>
+        <v>45302.531921296293</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -2595,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="12">
-        <v>45354.6875</v>
+        <v>45354.687881944446</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -2625,7 +2625,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12">
-        <v>45408.340277777781</v>
+        <v>45408.340810185182</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>47</v>
@@ -2655,7 +2655,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="12">
-        <v>45458.743055555555</v>
+        <v>45458.743333333332</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -2685,7 +2685,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="12">
-        <v>45480.607638888891</v>
+        <v>45480.608055555553</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
@@ -2715,7 +2715,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="12">
-        <v>45455.284722222219</v>
+        <v>45455.284930555557</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -2745,7 +2745,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="12">
-        <v>44951.552083333336</v>
+        <v>44951.552141203705</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>57</v>
@@ -2775,7 +2775,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="12">
-        <v>45002.489583333336</v>
+        <v>45002.490034722221</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -2805,7 +2805,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="12">
-        <v>45078.416666666664</v>
+        <v>45078.417256944442</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>53</v>
@@ -2835,7 +2835,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="12">
-        <v>45168.729166666664</v>
+        <v>45168.729328703703</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -2865,7 +2865,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="12">
-        <v>45218.319444444445</v>
+        <v>45218.319780092592</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -2895,7 +2895,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="12">
-        <v>45350.71875</v>
+        <v>45350.719236111108</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -2925,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="12">
-        <v>45418.725694444445</v>
+        <v>45418.726354166669</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -2955,7 +2955,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="12">
-        <v>45496.291666666664</v>
+        <v>45496.291701388887</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -2985,7 +2985,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="13">
-        <v>45422.739583333336</v>
+        <v>45422.739884259259</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -3013,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F197DD-EE87-4022-A4E6-1027B6E64DD6}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>44971.640277777777</v>
+        <v>44971.640451388892</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
@@ -3131,7 +3131,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="12">
-        <v>45055.40625</v>
+        <v>45055.40662037037</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -3175,7 +3175,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12">
-        <v>45128.729166666664</v>
+        <v>45128.729710648149</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -3219,7 +3219,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="12">
-        <v>45173.302083333336</v>
+        <v>45173.302187499998</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -3263,7 +3263,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="12">
-        <v>45248.708333333336</v>
+        <v>45248.70857638889</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -3307,7 +3307,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="12">
-        <v>45302.53125</v>
+        <v>45302.531921296293</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -3348,7 +3348,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="12">
-        <v>45354.6875</v>
+        <v>45354.687881944446</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12">
-        <v>45408.340277777781</v>
+        <v>45408.340810185182</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>47</v>
@@ -3430,7 +3430,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="12">
-        <v>45458.743055555555</v>
+        <v>45458.743333333332</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -3471,7 +3471,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="12">
-        <v>45480.607638888891</v>
+        <v>45480.608055555553</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
@@ -3512,7 +3512,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="12">
-        <v>45455.284722222219</v>
+        <v>45455.284930555557</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -3553,7 +3553,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="12">
-        <v>44951.552083333336</v>
+        <v>44951.552141203705</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>57</v>
@@ -3594,7 +3594,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="12">
-        <v>45002.489583333336</v>
+        <v>45002.490034722221</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -3635,7 +3635,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="12">
-        <v>45078.416666666664</v>
+        <v>45078.417256944442</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>53</v>
@@ -3676,7 +3676,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="12">
-        <v>45168.729166666664</v>
+        <v>45168.729328703703</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -3717,7 +3717,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="12">
-        <v>45218.319444444445</v>
+        <v>45218.319780092592</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -3758,7 +3758,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="12">
-        <v>45350.71875</v>
+        <v>45350.719236111108</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -3799,7 +3799,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="12">
-        <v>45418.725694444445</v>
+        <v>45418.726354166669</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -3840,7 +3840,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="12">
-        <v>45496.291666666664</v>
+        <v>45496.291701388887</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -3881,7 +3881,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="13">
-        <v>45422.739583333336</v>
+        <v>45422.739884259259</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>
@@ -3921,7 +3921,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3980,7 +3980,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>44971.640277777777</v>
+        <v>44971.640451388892</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
@@ -4018,7 +4018,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="12">
-        <v>45055.40625</v>
+        <v>45055.40662037037</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -4056,7 +4056,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12">
-        <v>45128.729166666664</v>
+        <v>45128.729710648149</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -4094,7 +4094,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="12">
-        <v>45173.302083333336</v>
+        <v>45173.302187499998</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
@@ -4132,7 +4132,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="12">
-        <v>45248.708333333336</v>
+        <v>45248.70857638889</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>41</v>
@@ -4170,7 +4170,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="12">
-        <v>45302.53125</v>
+        <v>45302.531921296293</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>47</v>
@@ -4208,7 +4208,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="12">
-        <v>45354.6875</v>
+        <v>45354.687881944446</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>59</v>
@@ -4246,7 +4246,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12">
-        <v>45408.340277777781</v>
+        <v>45408.340810185182</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>47</v>
@@ -4284,7 +4284,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="12">
-        <v>45458.743055555555</v>
+        <v>45458.743333333332</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
@@ -4322,7 +4322,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="12">
-        <v>45480.607638888891</v>
+        <v>45480.608055555553</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
@@ -4360,7 +4360,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="12">
-        <v>45455.284722222219</v>
+        <v>45455.284930555557</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>45</v>
@@ -4398,7 +4398,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="12">
-        <v>44951.552083333336</v>
+        <v>44951.552141203705</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>57</v>
@@ -4436,7 +4436,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="12">
-        <v>45002.489583333336</v>
+        <v>45002.490034722221</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -4474,7 +4474,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="12">
-        <v>45078.416666666664</v>
+        <v>45078.417256944442</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>53</v>
@@ -4512,7 +4512,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="12">
-        <v>45168.729166666664</v>
+        <v>45168.729328703703</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -4550,7 +4550,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="12">
-        <v>45218.319444444445</v>
+        <v>45218.319780092592</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -4588,7 +4588,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="12">
-        <v>45350.71875</v>
+        <v>45350.719236111108</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -4626,7 +4626,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="12">
-        <v>45418.725694444445</v>
+        <v>45418.726354166669</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>49</v>
@@ -4664,7 +4664,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="12">
-        <v>45496.291666666664</v>
+        <v>45496.291701388887</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -4702,7 +4702,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="13">
-        <v>45422.739583333336</v>
+        <v>45422.739884259259</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>41</v>

</xml_diff>